<commit_message>
v3 sent to Kevin 9/3/2019
</commit_message>
<xml_diff>
--- a/v2/dE.xlsx
+++ b/v2/dE.xlsx
@@ -362,204 +362,204 @@
         <v>0</v>
       </c>
       <c r="B1">
+        <v>33.55332124156859</v>
+      </c>
+      <c r="C1">
+        <v>39.681699737920887</v>
+      </c>
+      <c r="D1">
+        <v>43.049412492974781</v>
+      </c>
+      <c r="E1">
+        <v>101.20457063028111</v>
+      </c>
+      <c r="F1">
+        <v>76.636095618834176</v>
+      </c>
+      <c r="G1">
         <v>50.411404645068792</v>
       </c>
-      <c r="C1">
-        <v>74.084674794830306</v>
-      </c>
-      <c r="D1">
-        <v>90.38692880735222</v>
-      </c>
-      <c r="E1">
-        <v>85.547236149362135</v>
-      </c>
-      <c r="F1">
-        <v>50.40668473306804</v>
-      </c>
-      <c r="G1">
-        <v>54.893402085963551</v>
-      </c>
       <c r="H1">
-        <v>100</v>
+        <v>50.411404645068792</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>50.411404645068792</v>
+        <v>33.55332124156859</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
-        <v>39.166458843401074</v>
+        <v>19.842385248134388</v>
       </c>
       <c r="D2">
-        <v>82.18684105223403</v>
+        <v>84.666963306591285</v>
       </c>
       <c r="E2">
-        <v>67.811107314317837</v>
+        <v>96.712188291840633</v>
       </c>
       <c r="F2">
-        <v>51.386859288066105</v>
+        <v>62.917788541962778</v>
       </c>
       <c r="G2">
-        <v>40.133351765266603</v>
+        <v>43.983000151641612</v>
       </c>
       <c r="H2">
-        <v>45.810508977011068</v>
+        <v>43.983000151641612</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>74.084674794830306</v>
+        <v>39.681699737920887</v>
       </c>
       <c r="B3">
-        <v>39.166458843401074</v>
+        <v>19.842385248134388</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>39.337718084228278</v>
+        <v>62.656054087204915</v>
       </c>
       <c r="E3">
-        <v>48.510137102422441</v>
+        <v>103.42697049557917</v>
       </c>
       <c r="F3">
-        <v>62.384332860807042</v>
+        <v>66.412242282720399</v>
       </c>
       <c r="G3">
-        <v>69.058884083099286</v>
+        <v>52.881361297753301</v>
       </c>
       <c r="H3">
-        <v>31.977326471978717</v>
+        <v>52.881361297753301</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>90.38692880735222</v>
+        <v>43.049412492974781</v>
       </c>
       <c r="B4">
-        <v>82.18684105223403</v>
+        <v>84.666963306591285</v>
       </c>
       <c r="C4">
-        <v>39.337718084228278</v>
+        <v>62.656054087204915</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>39.253815791998903</v>
+        <v>43.863701646047936</v>
       </c>
       <c r="F4">
-        <v>72.58905875899012</v>
+        <v>51.136747775767461</v>
       </c>
       <c r="G4">
-        <v>105.62454164845346</v>
+        <v>72.182304891540497</v>
       </c>
       <c r="H4">
-        <v>32.300515826998833</v>
+        <v>72.182304891540497</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>85.547236149362135</v>
+        <v>101.20457063028111</v>
       </c>
       <c r="B5">
-        <v>67.811107314317837</v>
+        <v>96.712188291840633</v>
       </c>
       <c r="C5">
-        <v>48.510137102422441</v>
+        <v>103.42697049557917</v>
       </c>
       <c r="D5">
-        <v>39.253815791998903</v>
+        <v>43.863701646047936</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>39.192432990237101</v>
+        <v>32.83843964005483</v>
       </c>
       <c r="G5">
-        <v>61.564723913035522</v>
+        <v>64.30086530843441</v>
       </c>
       <c r="H5">
-        <v>25.56020430576103</v>
+        <v>64.30086530843441</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>50.40668473306804</v>
+        <v>76.636095618834176</v>
       </c>
       <c r="B6">
-        <v>51.386859288066105</v>
+        <v>62.917788541962778</v>
       </c>
       <c r="C6">
-        <v>62.384332860807042</v>
+        <v>66.412242282720399</v>
       </c>
       <c r="D6">
-        <v>72.58905875899012</v>
+        <v>51.136747775767461</v>
       </c>
       <c r="E6">
-        <v>39.192432990237101</v>
+        <v>32.83843964005483</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>39.33835816892352</v>
+        <v>31.155806452025956</v>
       </c>
       <c r="H6">
-        <v>41.309554391902353</v>
+        <v>31.155806452025956</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>54.893402085963551</v>
+        <v>50.411404645068792</v>
       </c>
       <c r="B7">
-        <v>40.133351765266603</v>
+        <v>43.983000151641612</v>
       </c>
       <c r="C7">
-        <v>69.058884083099286</v>
+        <v>52.881361297753301</v>
       </c>
       <c r="D7">
-        <v>105.62454164845346</v>
+        <v>72.182304891540497</v>
       </c>
       <c r="E7">
-        <v>61.564723913035522</v>
+        <v>64.30086530843441</v>
       </c>
       <c r="F7">
-        <v>39.33835816892352</v>
+        <v>31.155806452025956</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7">
-        <v>42.475651430646231</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>100</v>
+        <v>50.411404645068792</v>
       </c>
       <c r="B8">
-        <v>45.810508977011068</v>
+        <v>43.983000151641612</v>
       </c>
       <c r="C8">
-        <v>31.977326471978717</v>
+        <v>52.881361297753301</v>
       </c>
       <c r="D8">
-        <v>32.300515826998833</v>
+        <v>72.182304891540497</v>
       </c>
       <c r="E8">
-        <v>25.56020430576103</v>
+        <v>64.30086530843441</v>
       </c>
       <c r="F8">
-        <v>41.309554391902353</v>
+        <v>31.155806452025956</v>
       </c>
       <c r="G8">
-        <v>42.475651430646231</v>
+        <v>0</v>
       </c>
       <c r="H8">
         <v>0</v>

</xml_diff>

<commit_message>
v4 to calculate Kevin's proposal
</commit_message>
<xml_diff>
--- a/v2/dE.xlsx
+++ b/v2/dE.xlsx
@@ -362,204 +362,204 @@
         <v>0</v>
       </c>
       <c r="B1">
-        <v>33.55332124156859</v>
+        <v>37.852828665146504</v>
       </c>
       <c r="C1">
-        <v>39.681699737920887</v>
+        <v>32.085937424953364</v>
       </c>
       <c r="D1">
-        <v>43.049412492974781</v>
+        <v>27.609281693794845</v>
       </c>
       <c r="E1">
-        <v>101.20457063028111</v>
+        <v>43.465758266128674</v>
       </c>
       <c r="F1">
-        <v>76.636095618834176</v>
+        <v>31.159768996379047</v>
       </c>
       <c r="G1">
-        <v>50.411404645068792</v>
+        <v>31.196563288865786</v>
       </c>
       <c r="H1">
-        <v>50.411404645068792</v>
+        <v>33.238953705806018</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>33.55332124156859</v>
+        <v>37.852828665146504</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
-        <v>19.842385248134388</v>
+        <v>31.393557565474801</v>
       </c>
       <c r="D2">
-        <v>84.666963306591285</v>
+        <v>82.031182071948862</v>
       </c>
       <c r="E2">
-        <v>96.712188291840633</v>
+        <v>98.757015145876025</v>
       </c>
       <c r="F2">
-        <v>62.917788541962778</v>
+        <v>67.054214637777434</v>
       </c>
       <c r="G2">
-        <v>43.983000151641612</v>
+        <v>45.158836830976199</v>
       </c>
       <c r="H2">
-        <v>43.983000151641612</v>
+        <v>75.30387532858056</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>39.681699737920887</v>
+        <v>32.085937424953364</v>
       </c>
       <c r="B3">
-        <v>19.842385248134388</v>
+        <v>31.393557565474801</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>62.656054087204915</v>
+        <v>59.84370603723859</v>
       </c>
       <c r="E3">
-        <v>103.42697049557917</v>
+        <v>89.361466028965737</v>
       </c>
       <c r="F3">
-        <v>66.412242282720399</v>
+        <v>64.251603529056183</v>
       </c>
       <c r="G3">
-        <v>52.881361297753301</v>
+        <v>50.661003479774394</v>
       </c>
       <c r="H3">
-        <v>52.881361297753301</v>
+        <v>53.337692409187852</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>43.049412492974781</v>
+        <v>27.609281693794845</v>
       </c>
       <c r="B4">
-        <v>84.666963306591285</v>
+        <v>82.031182071948862</v>
       </c>
       <c r="C4">
-        <v>62.656054087204915</v>
+        <v>59.84370603723859</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>43.863701646047936</v>
+        <v>38.013632049814575</v>
       </c>
       <c r="F4">
-        <v>51.136747775767461</v>
+        <v>48.068914723611122</v>
       </c>
       <c r="G4">
-        <v>72.182304891540497</v>
+        <v>73.959778147718424</v>
       </c>
       <c r="H4">
-        <v>72.182304891540497</v>
+        <v>41.944401626694649</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>101.20457063028111</v>
+        <v>43.465758266128674</v>
       </c>
       <c r="B5">
-        <v>96.712188291840633</v>
+        <v>98.757015145876025</v>
       </c>
       <c r="C5">
-        <v>103.42697049557917</v>
+        <v>89.361466028965737</v>
       </c>
       <c r="D5">
-        <v>43.863701646047936</v>
+        <v>38.013632049814575</v>
       </c>
       <c r="E5">
         <v>0</v>
       </c>
       <c r="F5">
-        <v>32.83843964005483</v>
+        <v>33.619985515373834</v>
       </c>
       <c r="G5">
-        <v>64.30086530843441</v>
+        <v>63.130666499646544</v>
       </c>
       <c r="H5">
-        <v>64.30086530843441</v>
+        <v>30.441279634974393</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>76.636095618834176</v>
+        <v>31.159768996379047</v>
       </c>
       <c r="B6">
-        <v>62.917788541962778</v>
+        <v>67.054214637777434</v>
       </c>
       <c r="C6">
-        <v>66.412242282720399</v>
+        <v>64.251603529056183</v>
       </c>
       <c r="D6">
-        <v>51.136747775767461</v>
+        <v>48.068914723611122</v>
       </c>
       <c r="E6">
-        <v>32.83843964005483</v>
+        <v>33.619985515373834</v>
       </c>
       <c r="F6">
         <v>0</v>
       </c>
       <c r="G6">
-        <v>31.155806452025956</v>
+        <v>28.054480786641836</v>
       </c>
       <c r="H6">
-        <v>31.155806452025956</v>
+        <v>35.393328591758291</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>50.411404645068792</v>
+        <v>31.196563288865786</v>
       </c>
       <c r="B7">
-        <v>43.983000151641612</v>
+        <v>45.158836830976199</v>
       </c>
       <c r="C7">
-        <v>52.881361297753301</v>
+        <v>50.661003479774394</v>
       </c>
       <c r="D7">
-        <v>72.182304891540497</v>
+        <v>73.959778147718424</v>
       </c>
       <c r="E7">
-        <v>64.30086530843441</v>
+        <v>63.130666499646544</v>
       </c>
       <c r="F7">
-        <v>31.155806452025956</v>
+        <v>28.054480786641836</v>
       </c>
       <c r="G7">
         <v>0</v>
       </c>
       <c r="H7">
-        <v>0</v>
+        <v>45.810508977011068</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>50.411404645068792</v>
+        <v>33.238953705806018</v>
       </c>
       <c r="B8">
-        <v>43.983000151641612</v>
+        <v>75.30387532858056</v>
       </c>
       <c r="C8">
-        <v>52.881361297753301</v>
+        <v>53.337692409187852</v>
       </c>
       <c r="D8">
-        <v>72.182304891540497</v>
+        <v>41.944401626694649</v>
       </c>
       <c r="E8">
-        <v>64.30086530843441</v>
+        <v>30.441279634974393</v>
       </c>
       <c r="F8">
-        <v>31.155806452025956</v>
+        <v>35.393328591758291</v>
       </c>
       <c r="G8">
-        <v>0</v>
+        <v>45.810508977011068</v>
       </c>
       <c r="H8">
         <v>0</v>

</xml_diff>